<commit_message>
Add functionality for objects created from other acts
</commit_message>
<xml_diff>
--- a/tool/excels/handeling.xlsx
+++ b/tool/excels/handeling.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="118">
   <si>
     <t xml:space="preserve">act</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">[aanvraag]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">belanghebbende</t>
   </si>
   <si>
     <t xml:space="preserve">[aanvraag is geheel of gedeeltelijk geweigerd op grond van artikel 2:15 Awb]</t>
@@ -682,10 +679,10 @@
   </sheetPr>
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -827,7 +824,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="340" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="270.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -841,229 +838,229 @@
         <v>41</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>35</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="M8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="M9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1083,7 @@
   </sheetPr>
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1103,10 +1100,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,16 +1116,16 @@
     </row>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,14 +1134,14 @@
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="11" t="e">
         <f aca="false">VLOOKUP(C4,Handelingsframe!A2:M9882,1,0)</f>
         <v>#N/A</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="11" t="e">
         <f aca="false">VLOOKUP(G4,handelingsframe!#ref!,1,0)</f>
@@ -1160,7 +1157,7 @@
         <v>#N/A</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="13" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,2,0))="","",VLOOKUP(G4,handelingsframe!#ref!,2,0))</f>
@@ -1169,14 +1166,14 @@
     </row>
     <row r="8" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="13" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,3,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,3,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" s="13" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,3,0))="","",VLOOKUP(G4,handelingsframe!#ref!,3,0))</f>
@@ -1192,7 +1189,7 @@
         <v>#N/A</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" s="13" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,4,0))="","",VLOOKUP(G4,handelingsframe!#ref!,4,0))</f>
@@ -1201,14 +1198,14 @@
     </row>
     <row r="10" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="13" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,5,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,5,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G10" s="13" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,5,0))="","",VLOOKUP(G4,handelingsframe!#ref!,5,0))</f>
@@ -1217,14 +1214,14 @@
     </row>
     <row r="11" customFormat="false" ht="323" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="13" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,6,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,6,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="13" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,6,0))="","",VLOOKUP(G4,handelingsframe!#ref!,6,0))</f>
@@ -1233,14 +1230,14 @@
     </row>
     <row r="12" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="13" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,7,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,7,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G12" s="13" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,7,0))="","",VLOOKUP(G4,handelingsframe!#ref!,7,0))</f>
@@ -1249,14 +1246,14 @@
     </row>
     <row r="13" customFormat="false" ht="137" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="15" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,8,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,8,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" s="15" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,8,0))="","",VLOOKUP(G4,handelingsframe!#ref!,8,0))</f>
@@ -1265,24 +1262,24 @@
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="17"/>
       <c r="F14" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="19" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,9,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,9,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G15" s="19" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,9,0))="","",VLOOKUP(G4,handelingsframe!#ref!,9,0))</f>
@@ -1291,14 +1288,14 @@
     </row>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="19" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,10,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,10,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G16" s="19" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,10,0))="","",VLOOKUP(G4,handelingsframe!#ref!,10,0))</f>
@@ -1307,14 +1304,14 @@
     </row>
     <row r="17" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="19" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,11,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,11,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G17" s="19" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,11,0))="","",VLOOKUP(G4,handelingsframe!#ref!,11,0))</f>
@@ -1323,14 +1320,14 @@
     </row>
     <row r="18" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" s="19" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,12,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,12,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G18" s="19" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,12,0))="","",VLOOKUP(G4,handelingsframe!#ref!,12,0))</f>
@@ -1339,14 +1336,14 @@
     </row>
     <row r="19" customFormat="false" ht="238" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="19" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,13,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,13,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" s="19" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,13,0))="","",VLOOKUP(G4,handelingsframe!#ref!,13,0))</f>
@@ -1355,14 +1352,14 @@
     </row>
     <row r="20" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="19" t="e">
         <f aca="false">IF((VLOOKUP(C4,Handelingsframe!A2:M9882,14,0))="","",VLOOKUP(C4,Handelingsframe!A2:M9882,14,0))</f>
         <v>#VALUE!</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="19" t="e">
         <f aca="false">IF((VLOOKUP(G4,handelingsframe!#ref!,14,0))="","",VLOOKUP(G4,handelingsframe!#ref!,14,0))</f>

</xml_diff>